<commit_message>
Mejora en el diseño del dashboard del usuario y la seccion del bot brainbow
</commit_message>
<xml_diff>
--- a/public_html/assets/formatoBotBrainbow.xlsx
+++ b/public_html/assets/formatoBotBrainbow.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project_brainbow\public_html\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20430" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20430" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,9 +535,6 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
       <c r="B2" s="1">
         <v>41</v>
       </c>
@@ -558,9 +555,6 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6</v>
-      </c>
       <c r="B3" s="1">
         <v>41</v>
       </c>

</xml_diff>